<commit_message>
coomit at 2340 from home
</commit_message>
<xml_diff>
--- a/src/main/java/com/qtpselenium/app/salesforce/testdata/Suite.xlsx
+++ b/src/main/java/com/qtpselenium/app/salesforce/testdata/Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>TestCases</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>naveenv20</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://login.salesforce.com/?locale=ca</t>
   </si>
 </sst>
 </file>
@@ -165,6 +171,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -212,7 +221,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,7 +256,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,7 +491,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +514,9 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
@@ -518,6 +529,9 @@
       </c>
       <c r="C3" t="s">
         <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>